<commit_message>
added argument to not track documents that are blank as TRUE
</commit_message>
<xml_diff>
--- a/t_Batch.xlsx
+++ b/t_Batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://morningstaronline-my.sharepoint.com/personal/spencer_klug_pitchbook_com/Documents/India_PF_Expansion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_02F1510702721CDFEC4C5CD4475DCE3A874A9378" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CF133D5-0E55-4942-ACBC-EC78E036A0FF}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="11_3CA50A2AC14B36DFEC4C5CD4475DCE3A874AB8AC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E18A3A55-6F56-411E-B308-BE3AAC46E4CD}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-9690" yWindow="12165" windowWidth="19185" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AQ$501</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2882,12 +2893,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -2917,13 +2934,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3226,53 +3245,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AQ501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D138" sqref="D138"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="33" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="16.08984375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="17.81640625" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.6328125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="32" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="31.90625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.6328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="29.7265625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="33.26953125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="27.90625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="30.36328125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="28.6328125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="21" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="44.1796875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="39.6328125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="22.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.35">
@@ -3403,7 +3422,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>2500</v>
       </c>
@@ -3423,7 +3442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2501</v>
       </c>
@@ -3443,7 +3462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2502</v>
       </c>
@@ -3567,14 +3586,8 @@
       <c r="E7" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="2">
-        <v>44541</v>
-      </c>
       <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.35">
@@ -3593,14 +3606,8 @@
       <c r="E8" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="2">
-        <v>44541</v>
-      </c>
       <c r="G8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.35">
@@ -3619,14 +3626,8 @@
       <c r="E9" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="2">
-        <v>44541</v>
-      </c>
       <c r="G9" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.35">
@@ -3645,14 +3646,8 @@
       <c r="E10" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="2">
-        <v>44541</v>
-      </c>
       <c r="G10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.35">
@@ -3671,14 +3666,8 @@
       <c r="E11" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="2">
-        <v>44541</v>
-      </c>
       <c r="G11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="3">
-        <v>42460</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.35">
@@ -3803,14 +3792,8 @@
       <c r="E14" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="2">
-        <v>44541</v>
-      </c>
       <c r="G14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="3">
-        <v>40268</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.35">
@@ -3873,14 +3856,8 @@
       <c r="E16" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="2">
-        <v>44541</v>
-      </c>
       <c r="G16" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" s="3">
-        <v>42094</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.35">
@@ -4276,7 +4253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2518</v>
       </c>
@@ -4296,7 +4273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>2519</v>
       </c>
@@ -4316,7 +4293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2520</v>
       </c>
@@ -4336,7 +4313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>2521</v>
       </c>
@@ -4527,7 +4504,7 @@
         <v>88763308</v>
       </c>
     </row>
-    <row r="27" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>2525</v>
       </c>
@@ -4547,7 +4524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>2526</v>
       </c>
@@ -4567,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>2527</v>
       </c>
@@ -4587,7 +4564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>2528</v>
       </c>
@@ -4667,14 +4644,8 @@
       <c r="E32" t="s">
         <v>90</v>
       </c>
-      <c r="F32" s="2">
-        <v>44541</v>
-      </c>
       <c r="G32" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" s="3">
-        <v>39172</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:43" x14ac:dyDescent="0.35">
@@ -4721,7 +4692,7 @@
         <v>-49399460</v>
       </c>
     </row>
-    <row r="34" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>2532</v>
       </c>
@@ -4757,14 +4728,8 @@
       <c r="E35" t="s">
         <v>103</v>
       </c>
-      <c r="F35" s="2">
-        <v>44541</v>
-      </c>
       <c r="G35" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:43" x14ac:dyDescent="0.35">
@@ -4783,14 +4748,8 @@
       <c r="E36" t="s">
         <v>105</v>
       </c>
-      <c r="F36" s="2">
-        <v>44541</v>
-      </c>
       <c r="G36" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" s="3">
-        <v>43830</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:43" x14ac:dyDescent="0.35">
@@ -4809,14 +4768,8 @@
       <c r="E37" t="s">
         <v>107</v>
       </c>
-      <c r="F37" s="2">
-        <v>44541</v>
-      </c>
       <c r="G37" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:43" x14ac:dyDescent="0.35">
@@ -4835,14 +4788,8 @@
       <c r="E38" t="s">
         <v>109</v>
       </c>
-      <c r="F38" s="2">
-        <v>44541</v>
-      </c>
       <c r="G38" t="b">
-        <v>1</v>
-      </c>
-      <c r="H38" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:43" x14ac:dyDescent="0.35">
@@ -4861,14 +4808,8 @@
       <c r="E39" t="s">
         <v>111</v>
       </c>
-      <c r="F39" s="2">
-        <v>44541</v>
-      </c>
       <c r="G39" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" s="3">
-        <v>44196</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:43" x14ac:dyDescent="0.35">
@@ -5005,14 +4946,8 @@
       <c r="E42" t="s">
         <v>117</v>
       </c>
-      <c r="F42" s="2">
-        <v>44541</v>
-      </c>
       <c r="G42" t="b">
-        <v>1</v>
-      </c>
-      <c r="H42" s="3">
-        <v>42460</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:43" x14ac:dyDescent="0.35">
@@ -5908,82 +5843,92 @@
       <c r="G51" t="b">
         <v>1</v>
       </c>
-      <c r="H51" s="3">
+      <c r="H51" s="4">
         <v>41729</v>
       </c>
-      <c r="O51">
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5">
         <v>11208133</v>
       </c>
-      <c r="P51">
+      <c r="P51" s="5">
         <v>5900000</v>
       </c>
-      <c r="Q51">
+      <c r="Q51" s="5">
         <v>416</v>
       </c>
-      <c r="R51">
-        <v>0</v>
-      </c>
-      <c r="S51">
+      <c r="R51" s="5">
+        <v>0</v>
+      </c>
+      <c r="S51" s="5">
         <v>11137897</v>
       </c>
-      <c r="T51">
+      <c r="T51" s="5">
         <v>14725223</v>
       </c>
-      <c r="U51">
-        <v>0</v>
-      </c>
-      <c r="V51">
-        <v>0</v>
-      </c>
-      <c r="W51">
-        <v>0</v>
-      </c>
-      <c r="X51">
-        <v>0</v>
-      </c>
-      <c r="Y51">
+      <c r="U51" s="5">
+        <v>0</v>
+      </c>
+      <c r="V51" s="5">
+        <v>0</v>
+      </c>
+      <c r="W51" s="5">
+        <v>0</v>
+      </c>
+      <c r="X51" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y51" s="5">
         <v>854000</v>
       </c>
-      <c r="Z51">
+      <c r="Z51" s="5">
         <v>30538062</v>
       </c>
-      <c r="AE51">
+      <c r="AA51" s="5"/>
+      <c r="AB51" s="5"/>
+      <c r="AC51" s="5"/>
+      <c r="AD51" s="5"/>
+      <c r="AE51" s="5">
         <v>7350000</v>
       </c>
-      <c r="AF51">
-        <v>0</v>
-      </c>
-      <c r="AG51">
-        <v>0</v>
-      </c>
-      <c r="AH51">
+      <c r="AF51" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG51" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH51" s="5">
         <v>1352701</v>
       </c>
-      <c r="AI51">
+      <c r="AI51" s="5">
         <v>236770</v>
       </c>
-      <c r="AJ51">
+      <c r="AJ51" s="5">
         <v>4490042</v>
       </c>
-      <c r="AK51">
-        <v>0</v>
-      </c>
-      <c r="AL51">
+      <c r="AK51" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL51" s="5">
         <v>429109</v>
       </c>
-      <c r="AM51">
-        <v>0</v>
-      </c>
-      <c r="AN51">
-        <v>0</v>
-      </c>
-      <c r="AO51">
-        <v>0</v>
-      </c>
-      <c r="AP51">
-        <v>0</v>
-      </c>
-      <c r="AQ51">
+      <c r="AM51" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN51" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO51" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP51" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ51" s="5">
         <v>3391833</v>
       </c>
     </row>
@@ -6009,82 +5954,92 @@
       <c r="G52" t="b">
         <v>1</v>
       </c>
-      <c r="H52" s="3">
+      <c r="H52" s="4">
         <v>41364</v>
       </c>
-      <c r="O52">
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5">
         <v>6541599</v>
       </c>
-      <c r="P52">
+      <c r="P52" s="5">
         <v>4500000</v>
       </c>
-      <c r="Q52">
+      <c r="Q52" s="5">
         <v>2266</v>
       </c>
-      <c r="R52">
-        <v>0</v>
-      </c>
-      <c r="S52">
+      <c r="R52" s="5">
+        <v>0</v>
+      </c>
+      <c r="S52" s="5">
         <v>8073345</v>
       </c>
-      <c r="T52">
+      <c r="T52" s="5">
         <v>12109</v>
       </c>
-      <c r="U52">
-        <v>0</v>
-      </c>
-      <c r="V52">
-        <v>0</v>
-      </c>
-      <c r="W52">
-        <v>0</v>
-      </c>
-      <c r="X52">
-        <v>0</v>
-      </c>
-      <c r="Y52">
+      <c r="U52" s="5">
+        <v>0</v>
+      </c>
+      <c r="V52" s="5">
+        <v>0</v>
+      </c>
+      <c r="W52" s="5">
+        <v>0</v>
+      </c>
+      <c r="X52" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y52" s="5">
         <v>15512069</v>
       </c>
-      <c r="Z52">
+      <c r="Z52" s="5">
         <v>24577354</v>
       </c>
-      <c r="AE52">
+      <c r="AA52" s="5"/>
+      <c r="AB52" s="5"/>
+      <c r="AC52" s="5"/>
+      <c r="AD52" s="5"/>
+      <c r="AE52" s="5">
         <v>9350000</v>
       </c>
-      <c r="AF52">
-        <v>0</v>
-      </c>
-      <c r="AG52">
-        <v>0</v>
-      </c>
-      <c r="AH52">
+      <c r="AF52" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG52" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH52" s="5">
         <v>1072153</v>
       </c>
-      <c r="AI52">
+      <c r="AI52" s="5">
         <v>304907</v>
       </c>
-      <c r="AJ52">
+      <c r="AJ52" s="5">
         <v>2806429</v>
       </c>
-      <c r="AK52">
-        <v>0</v>
-      </c>
-      <c r="AL52">
+      <c r="AK52" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL52" s="5">
         <v>422935</v>
       </c>
-      <c r="AM52">
-        <v>0</v>
-      </c>
-      <c r="AN52">
-        <v>0</v>
-      </c>
-      <c r="AO52">
-        <v>0</v>
-      </c>
-      <c r="AP52">
-        <v>0</v>
-      </c>
-      <c r="AQ52">
+      <c r="AM52" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN52" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO52" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP52" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ52" s="5">
         <v>556896</v>
       </c>
     </row>
@@ -6411,14 +6366,8 @@
       <c r="E58" t="s">
         <v>147</v>
       </c>
-      <c r="F58" s="2">
-        <v>44541</v>
-      </c>
       <c r="G58" t="b">
-        <v>1</v>
-      </c>
-      <c r="H58" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:43" x14ac:dyDescent="0.35">
@@ -6437,14 +6386,8 @@
       <c r="E59" t="s">
         <v>149</v>
       </c>
-      <c r="F59" s="2">
-        <v>44541</v>
-      </c>
       <c r="G59" t="b">
-        <v>1</v>
-      </c>
-      <c r="H59" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:43" x14ac:dyDescent="0.35">
@@ -6463,14 +6406,8 @@
       <c r="E60" t="s">
         <v>151</v>
       </c>
-      <c r="F60" s="2">
-        <v>44541</v>
-      </c>
       <c r="G60" t="b">
-        <v>1</v>
-      </c>
-      <c r="H60" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:43" x14ac:dyDescent="0.35">
@@ -7007,14 +6944,8 @@
       <c r="E65" t="s">
         <v>147</v>
       </c>
-      <c r="F65" s="2">
-        <v>44541</v>
-      </c>
       <c r="G65" t="b">
-        <v>1</v>
-      </c>
-      <c r="H65" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:43" x14ac:dyDescent="0.35">
@@ -7601,14 +7532,8 @@
       <c r="E74" t="s">
         <v>165</v>
       </c>
-      <c r="F74" s="2">
-        <v>44541</v>
-      </c>
       <c r="G74" t="b">
-        <v>1</v>
-      </c>
-      <c r="H74" s="3">
-        <v>40633</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:43" x14ac:dyDescent="0.35">
@@ -8161,14 +8086,8 @@
       <c r="E81" t="s">
         <v>186</v>
       </c>
-      <c r="F81" s="2">
-        <v>44541</v>
-      </c>
       <c r="G81" t="b">
-        <v>1</v>
-      </c>
-      <c r="H81" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:43" x14ac:dyDescent="0.35">
@@ -8187,14 +8106,8 @@
       <c r="E82" t="s">
         <v>188</v>
       </c>
-      <c r="F82" s="2">
-        <v>44541</v>
-      </c>
       <c r="G82" t="b">
-        <v>1</v>
-      </c>
-      <c r="H82" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:43" x14ac:dyDescent="0.35">
@@ -8734,14 +8647,8 @@
       <c r="E87" t="s">
         <v>197</v>
       </c>
-      <c r="F87" s="2">
-        <v>44541</v>
-      </c>
       <c r="G87" t="b">
-        <v>1</v>
-      </c>
-      <c r="H87" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:43" x14ac:dyDescent="0.35">
@@ -8760,14 +8667,8 @@
       <c r="E88" t="s">
         <v>199</v>
       </c>
-      <c r="F88" s="2">
-        <v>44541</v>
-      </c>
       <c r="G88" t="b">
-        <v>1</v>
-      </c>
-      <c r="H88" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:43" x14ac:dyDescent="0.35">
@@ -8786,14 +8687,8 @@
       <c r="E89" t="s">
         <v>201</v>
       </c>
-      <c r="F89" s="2">
-        <v>44541</v>
-      </c>
       <c r="G89" t="b">
-        <v>1</v>
-      </c>
-      <c r="H89" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:43" x14ac:dyDescent="0.35">
@@ -10144,7 +10039,7 @@
         <v>21151</v>
       </c>
     </row>
-    <row r="101" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>2599</v>
       </c>
@@ -10164,7 +10059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>2600</v>
       </c>
@@ -10184,7 +10079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>2601</v>
       </c>
@@ -10220,14 +10115,8 @@
       <c r="E104" t="s">
         <v>232</v>
       </c>
-      <c r="F104" s="2">
-        <v>44541</v>
-      </c>
       <c r="G104" t="b">
-        <v>1</v>
-      </c>
-      <c r="H104" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:43" x14ac:dyDescent="0.35">
@@ -10246,14 +10135,8 @@
       <c r="E105" t="s">
         <v>234</v>
       </c>
-      <c r="F105" s="2">
-        <v>44541</v>
-      </c>
       <c r="G105" t="b">
-        <v>1</v>
-      </c>
-      <c r="H105" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:43" x14ac:dyDescent="0.35">
@@ -10272,14 +10155,8 @@
       <c r="E106" t="s">
         <v>236</v>
       </c>
-      <c r="F106" s="2">
-        <v>44541</v>
-      </c>
       <c r="G106" t="b">
-        <v>1</v>
-      </c>
-      <c r="H106" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:43" x14ac:dyDescent="0.35">
@@ -10298,14 +10175,8 @@
       <c r="E107" t="s">
         <v>238</v>
       </c>
-      <c r="F107" s="2">
-        <v>44541</v>
-      </c>
       <c r="G107" t="b">
-        <v>1</v>
-      </c>
-      <c r="H107" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:43" x14ac:dyDescent="0.35">
@@ -10484,14 +10355,8 @@
       <c r="E110" t="s">
         <v>244</v>
       </c>
-      <c r="F110" s="2">
-        <v>44541</v>
-      </c>
       <c r="G110" t="b">
-        <v>1</v>
-      </c>
-      <c r="H110" s="3">
-        <v>42460</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:43" x14ac:dyDescent="0.35">
@@ -11160,14 +11025,8 @@
       <c r="E118" t="s">
         <v>261</v>
       </c>
-      <c r="F118" s="2">
-        <v>44541</v>
-      </c>
       <c r="G118" t="b">
-        <v>1</v>
-      </c>
-      <c r="H118" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:43" x14ac:dyDescent="0.35">
@@ -11186,14 +11045,8 @@
       <c r="E119" t="s">
         <v>223</v>
       </c>
-      <c r="F119" s="2">
-        <v>44541</v>
-      </c>
       <c r="G119" t="b">
-        <v>1</v>
-      </c>
-      <c r="H119" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:43" x14ac:dyDescent="0.35">
@@ -11212,14 +11065,8 @@
       <c r="E120" t="s">
         <v>264</v>
       </c>
-      <c r="F120" s="2">
-        <v>44541</v>
-      </c>
       <c r="G120" t="b">
-        <v>1</v>
-      </c>
-      <c r="H120" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:43" x14ac:dyDescent="0.35">
@@ -11735,42 +11582,66 @@
       <c r="G125" t="b">
         <v>1</v>
       </c>
-      <c r="H125" s="3">
+      <c r="H125" s="4">
         <v>39538</v>
       </c>
-      <c r="L125">
+      <c r="I125" s="5"/>
+      <c r="J125" s="5"/>
+      <c r="K125" s="5"/>
+      <c r="L125" s="5">
         <v>63887</v>
       </c>
-      <c r="O125">
-        <v>0</v>
-      </c>
-      <c r="P125">
+      <c r="M125" s="5"/>
+      <c r="N125" s="5"/>
+      <c r="O125" s="5">
+        <v>0</v>
+      </c>
+      <c r="P125" s="5">
         <v>7045953</v>
       </c>
-      <c r="R125">
-        <v>0</v>
-      </c>
-      <c r="T125">
+      <c r="Q125" s="5"/>
+      <c r="R125" s="5">
+        <v>0</v>
+      </c>
+      <c r="S125" s="5"/>
+      <c r="T125" s="5">
         <v>27941</v>
       </c>
-      <c r="V125">
+      <c r="U125" s="5"/>
+      <c r="V125" s="5">
         <v>4676011</v>
       </c>
-      <c r="W125">
-        <v>0</v>
-      </c>
-      <c r="X125">
-        <v>0</v>
-      </c>
-      <c r="Y125">
+      <c r="W125" s="5">
+        <v>0</v>
+      </c>
+      <c r="X125" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y125" s="5">
         <v>1008786</v>
       </c>
-      <c r="Z125">
+      <c r="Z125" s="5">
         <v>7045953</v>
       </c>
-      <c r="AO125">
-        <v>0</v>
-      </c>
+      <c r="AA125" s="5"/>
+      <c r="AB125" s="5"/>
+      <c r="AC125" s="5"/>
+      <c r="AD125" s="5"/>
+      <c r="AE125" s="5"/>
+      <c r="AF125" s="5"/>
+      <c r="AG125" s="5"/>
+      <c r="AH125" s="5"/>
+      <c r="AI125" s="5"/>
+      <c r="AJ125" s="5"/>
+      <c r="AK125" s="5"/>
+      <c r="AL125" s="5"/>
+      <c r="AM125" s="5"/>
+      <c r="AN125" s="5"/>
+      <c r="AO125" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP125" s="5"/>
+      <c r="AQ125" s="5"/>
     </row>
     <row r="126" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
@@ -12499,14 +12370,8 @@
       <c r="E138" t="s">
         <v>293</v>
       </c>
-      <c r="F138" s="2">
-        <v>44541</v>
-      </c>
       <c r="G138" t="b">
-        <v>1</v>
-      </c>
-      <c r="H138" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:43" x14ac:dyDescent="0.35">
@@ -12525,14 +12390,8 @@
       <c r="E139" t="s">
         <v>295</v>
       </c>
-      <c r="F139" s="2">
-        <v>44541</v>
-      </c>
       <c r="G139" t="b">
-        <v>1</v>
-      </c>
-      <c r="H139" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:43" x14ac:dyDescent="0.35">
@@ -12551,14 +12410,8 @@
       <c r="E140" t="s">
         <v>297</v>
       </c>
-      <c r="F140" s="2">
-        <v>44541</v>
-      </c>
       <c r="G140" t="b">
-        <v>1</v>
-      </c>
-      <c r="H140" s="3">
-        <v>42460</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:43" x14ac:dyDescent="0.35">
@@ -12577,14 +12430,8 @@
       <c r="E141" t="s">
         <v>105</v>
       </c>
-      <c r="F141" s="2">
-        <v>44541</v>
-      </c>
       <c r="G141" t="b">
-        <v>1</v>
-      </c>
-      <c r="H141" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:43" x14ac:dyDescent="0.35">
@@ -12603,14 +12450,8 @@
       <c r="E142" t="s">
         <v>300</v>
       </c>
-      <c r="F142" s="2">
-        <v>44541</v>
-      </c>
       <c r="G142" t="b">
-        <v>1</v>
-      </c>
-      <c r="H142" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:43" x14ac:dyDescent="0.35">
@@ -13219,14 +13060,8 @@
       <c r="E150" t="s">
         <v>317</v>
       </c>
-      <c r="F150" s="2">
-        <v>44541</v>
-      </c>
       <c r="G150" t="b">
-        <v>1</v>
-      </c>
-      <c r="H150" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:43" x14ac:dyDescent="0.35">
@@ -13245,14 +13080,8 @@
       <c r="E151" t="s">
         <v>319</v>
       </c>
-      <c r="F151" s="2">
-        <v>44541</v>
-      </c>
       <c r="G151" t="b">
-        <v>1</v>
-      </c>
-      <c r="H151" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:43" x14ac:dyDescent="0.35">
@@ -13271,14 +13100,8 @@
       <c r="E152" t="s">
         <v>321</v>
       </c>
-      <c r="F152" s="2">
-        <v>44541</v>
-      </c>
       <c r="G152" t="b">
-        <v>1</v>
-      </c>
-      <c r="H152" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:43" x14ac:dyDescent="0.35">
@@ -13297,14 +13120,8 @@
       <c r="E153" t="s">
         <v>323</v>
       </c>
-      <c r="F153" s="2">
-        <v>44541</v>
-      </c>
       <c r="G153" t="b">
-        <v>1</v>
-      </c>
-      <c r="H153" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:43" x14ac:dyDescent="0.35">
@@ -13552,17 +13369,11 @@
       <c r="E156" t="s">
         <v>62</v>
       </c>
-      <c r="F156" s="2">
-        <v>44541</v>
-      </c>
       <c r="G156" t="b">
-        <v>1</v>
-      </c>
-      <c r="H156" s="3">
-        <v>42460</v>
-      </c>
-    </row>
-    <row r="157" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>2655</v>
       </c>
@@ -13582,7 +13393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>2656</v>
       </c>
@@ -13602,7 +13413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>2657</v>
       </c>
@@ -13622,7 +13433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>2658</v>
       </c>
@@ -13860,7 +13671,7 @@
         <v>3682587</v>
       </c>
     </row>
-    <row r="165" spans="1:41" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>2663</v>
       </c>
@@ -13880,7 +13691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:41" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
         <v>2664</v>
       </c>
@@ -13900,7 +13711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:41" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
         <v>2665</v>
       </c>
@@ -13920,7 +13731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:41" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
         <v>2666</v>
       </c>
@@ -14116,7 +13927,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="173" spans="1:41" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
         <v>2671</v>
       </c>
@@ -14136,7 +13947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:41" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
         <v>2672</v>
       </c>
@@ -14172,14 +13983,8 @@
       <c r="E175" t="s">
         <v>357</v>
       </c>
-      <c r="F175" s="2">
-        <v>44541</v>
-      </c>
       <c r="G175" t="b">
-        <v>1</v>
-      </c>
-      <c r="H175" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:41" x14ac:dyDescent="0.35">
@@ -14198,14 +14003,8 @@
       <c r="E176" t="s">
         <v>359</v>
       </c>
-      <c r="F176" s="2">
-        <v>44541</v>
-      </c>
       <c r="G176" t="b">
-        <v>1</v>
-      </c>
-      <c r="H176" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:43" x14ac:dyDescent="0.35">
@@ -14224,14 +14023,8 @@
       <c r="E177" t="s">
         <v>361</v>
       </c>
-      <c r="F177" s="2">
-        <v>44541</v>
-      </c>
       <c r="G177" t="b">
-        <v>1</v>
-      </c>
-      <c r="H177" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:43" x14ac:dyDescent="0.35">
@@ -14250,14 +14043,8 @@
       <c r="E178" t="s">
         <v>182</v>
       </c>
-      <c r="F178" s="2">
-        <v>44541</v>
-      </c>
       <c r="G178" t="b">
-        <v>1</v>
-      </c>
-      <c r="H178" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:43" x14ac:dyDescent="0.35">
@@ -14276,14 +14063,8 @@
       <c r="E179" t="s">
         <v>364</v>
       </c>
-      <c r="F179" s="2">
-        <v>44541</v>
-      </c>
       <c r="G179" t="b">
-        <v>1</v>
-      </c>
-      <c r="H179" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:43" x14ac:dyDescent="0.35">
@@ -14411,14 +14192,8 @@
       <c r="E182" t="s">
         <v>370</v>
       </c>
-      <c r="F182" s="2">
-        <v>44541</v>
-      </c>
       <c r="G182" t="b">
-        <v>1</v>
-      </c>
-      <c r="H182" s="3">
-        <v>42460</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183" spans="1:43" x14ac:dyDescent="0.35">
@@ -14437,14 +14212,8 @@
       <c r="E183" t="s">
         <v>366</v>
       </c>
-      <c r="F183" s="2">
-        <v>44541</v>
-      </c>
       <c r="G183" t="b">
-        <v>1</v>
-      </c>
-      <c r="H183" s="3">
-        <v>40268</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184" spans="1:43" x14ac:dyDescent="0.35">
@@ -15689,112 +15458,112 @@
       <c r="G194" t="b">
         <v>1</v>
       </c>
-      <c r="H194" s="3">
+      <c r="H194" s="4">
         <v>43921</v>
       </c>
-      <c r="I194">
+      <c r="I194" s="5">
         <v>38694841</v>
       </c>
-      <c r="J194">
+      <c r="J194" s="5">
         <v>-119064331</v>
       </c>
-      <c r="K194">
+      <c r="K194" s="5">
         <v>40589805</v>
       </c>
-      <c r="L194">
+      <c r="L194" s="5">
         <v>5247474</v>
       </c>
-      <c r="M194">
+      <c r="M194" s="5">
         <v>157759172</v>
       </c>
-      <c r="N194">
-        <v>0</v>
-      </c>
-      <c r="O194">
+      <c r="N194" s="5">
+        <v>0</v>
+      </c>
+      <c r="O194" s="5">
         <v>-4614753</v>
       </c>
-      <c r="P194">
+      <c r="P194" s="5">
         <v>129658000</v>
       </c>
-      <c r="Q194">
-        <v>0</v>
-      </c>
-      <c r="R194">
+      <c r="Q194" s="5">
+        <v>0</v>
+      </c>
+      <c r="R194" s="5">
         <v>30639700</v>
       </c>
-      <c r="S194">
-        <v>0</v>
-      </c>
-      <c r="T194">
+      <c r="S194" s="5">
+        <v>0</v>
+      </c>
+      <c r="T194" s="5">
         <v>35969226</v>
       </c>
-      <c r="U194">
+      <c r="U194" s="5">
         <v>31097085</v>
       </c>
-      <c r="V194">
-        <v>0</v>
-      </c>
-      <c r="W194">
-        <v>0</v>
-      </c>
-      <c r="X194">
+      <c r="V194" s="5">
+        <v>0</v>
+      </c>
+      <c r="W194" s="5">
+        <v>0</v>
+      </c>
+      <c r="X194" s="5">
         <v>44410939</v>
       </c>
-      <c r="Y194">
-        <v>0</v>
-      </c>
-      <c r="Z194">
+      <c r="Y194" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z194" s="5">
         <v>748458032</v>
       </c>
-      <c r="AA194">
-        <v>0</v>
-      </c>
-      <c r="AB194">
+      <c r="AA194" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB194" s="5">
         <v>73849143</v>
       </c>
-      <c r="AC194">
-        <v>0</v>
-      </c>
-      <c r="AD194">
+      <c r="AC194" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD194" s="5">
         <v>-119064331</v>
       </c>
-      <c r="AE194">
-        <v>0</v>
-      </c>
-      <c r="AF194">
+      <c r="AE194" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF194" s="5">
         <v>2500000</v>
       </c>
-      <c r="AG194">
+      <c r="AG194" s="5">
         <v>2234627</v>
       </c>
-      <c r="AH194">
+      <c r="AH194" s="5">
         <v>78141480</v>
       </c>
-      <c r="AI194">
+      <c r="AI194" s="5">
         <v>1357582</v>
       </c>
-      <c r="AJ194">
+      <c r="AJ194" s="5">
         <v>316338786</v>
       </c>
-      <c r="AK194">
+      <c r="AK194" s="5">
         <v>222842310</v>
       </c>
-      <c r="AL194">
+      <c r="AL194" s="5">
         <v>9519147</v>
       </c>
-      <c r="AM194">
+      <c r="AM194" s="5">
         <v>106936</v>
       </c>
-      <c r="AN194">
-        <v>0</v>
-      </c>
-      <c r="AO194">
-        <v>0</v>
-      </c>
-      <c r="AP194">
+      <c r="AN194" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO194" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP194" s="5">
         <v>70909600</v>
       </c>
-      <c r="AQ194">
+      <c r="AQ194" s="5">
         <v>525805399</v>
       </c>
     </row>
@@ -16522,7 +16291,7 @@
         <v>10908968</v>
       </c>
     </row>
-    <row r="206" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A206" s="1">
         <v>2704</v>
       </c>
@@ -16542,7 +16311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A207" s="1">
         <v>2705</v>
       </c>
@@ -16562,7 +16331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A208" s="1">
         <v>2706</v>
       </c>
@@ -16582,7 +16351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A209" s="1">
         <v>2707</v>
       </c>
@@ -16602,7 +16371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A210" s="1">
         <v>2708</v>
       </c>
@@ -16622,7 +16391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A211" s="1">
         <v>2709</v>
       </c>
@@ -16642,7 +16411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A212" s="1">
         <v>2710</v>
       </c>
@@ -16662,7 +16431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A213" s="1">
         <v>2711</v>
       </c>
@@ -16682,7 +16451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A214" s="1">
         <v>2712</v>
       </c>
@@ -16718,14 +16487,8 @@
       <c r="E215" t="s">
         <v>427</v>
       </c>
-      <c r="F215" s="2">
-        <v>44541</v>
-      </c>
       <c r="G215" t="b">
-        <v>1</v>
-      </c>
-      <c r="H215" s="3">
-        <v>42460</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216" spans="1:43" x14ac:dyDescent="0.35">
@@ -16838,14 +16601,8 @@
       <c r="E218" t="s">
         <v>434</v>
       </c>
-      <c r="F218" s="2">
-        <v>44541</v>
-      </c>
       <c r="G218" t="b">
-        <v>1</v>
-      </c>
-      <c r="H218" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="219" spans="1:43" x14ac:dyDescent="0.35">
@@ -16864,14 +16621,8 @@
       <c r="E219" t="s">
         <v>436</v>
       </c>
-      <c r="F219" s="2">
-        <v>44541</v>
-      </c>
       <c r="G219" t="b">
-        <v>1</v>
-      </c>
-      <c r="H219" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:43" x14ac:dyDescent="0.35">
@@ -16890,14 +16641,8 @@
       <c r="E220" t="s">
         <v>438</v>
       </c>
-      <c r="F220" s="2">
-        <v>44541</v>
-      </c>
       <c r="G220" t="b">
-        <v>1</v>
-      </c>
-      <c r="H220" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221" spans="1:43" x14ac:dyDescent="0.35">
@@ -16916,14 +16661,8 @@
       <c r="E221" t="s">
         <v>440</v>
       </c>
-      <c r="F221" s="2">
-        <v>44541</v>
-      </c>
       <c r="G221" t="b">
-        <v>1</v>
-      </c>
-      <c r="H221" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222" spans="1:43" x14ac:dyDescent="0.35">
@@ -18171,7 +17910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A234" s="1">
         <v>2732</v>
       </c>
@@ -18191,7 +17930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A235" s="1">
         <v>2733</v>
       </c>
@@ -18211,7 +17950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A236" s="1">
         <v>2734</v>
       </c>
@@ -18231,7 +17970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A237" s="1">
         <v>2735</v>
       </c>
@@ -18310,7 +18049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A239" s="1">
         <v>2737</v>
       </c>
@@ -18330,7 +18069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A240" s="1">
         <v>2738</v>
       </c>
@@ -18350,7 +18089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:41" hidden="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A241" s="1">
         <v>2739</v>
       </c>
@@ -18370,7 +18109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:41" hidden="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A242" s="1">
         <v>2740</v>
       </c>
@@ -18434,7 +18173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:41" hidden="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A244" s="1">
         <v>2742</v>
       </c>
@@ -18470,14 +18209,8 @@
       <c r="E245" t="s">
         <v>482</v>
       </c>
-      <c r="F245" s="2">
-        <v>44541</v>
-      </c>
       <c r="G245" t="b">
-        <v>1</v>
-      </c>
-      <c r="H245" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="246" spans="1:41" x14ac:dyDescent="0.35">
@@ -18496,14 +18229,8 @@
       <c r="E246" t="s">
         <v>484</v>
       </c>
-      <c r="F246" s="2">
-        <v>44541</v>
-      </c>
       <c r="G246" t="b">
-        <v>1</v>
-      </c>
-      <c r="H246" s="3">
-        <v>44286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="247" spans="1:41" x14ac:dyDescent="0.35">
@@ -18522,14 +18249,8 @@
       <c r="E247" t="s">
         <v>486</v>
       </c>
-      <c r="F247" s="2">
-        <v>44541</v>
-      </c>
       <c r="G247" t="b">
-        <v>1</v>
-      </c>
-      <c r="H247" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="248" spans="1:41" x14ac:dyDescent="0.35">
@@ -18548,14 +18269,8 @@
       <c r="E248" t="s">
         <v>488</v>
       </c>
-      <c r="F248" s="2">
-        <v>44541</v>
-      </c>
       <c r="G248" t="b">
-        <v>1</v>
-      </c>
-      <c r="H248" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="249" spans="1:41" x14ac:dyDescent="0.35">
@@ -18574,14 +18289,8 @@
       <c r="E249" t="s">
         <v>490</v>
       </c>
-      <c r="F249" s="2">
-        <v>44541</v>
-      </c>
       <c r="G249" t="b">
-        <v>1</v>
-      </c>
-      <c r="H249" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250" spans="1:41" x14ac:dyDescent="0.35">
@@ -18600,14 +18309,8 @@
       <c r="E250" t="s">
         <v>492</v>
       </c>
-      <c r="F250" s="2">
-        <v>44541</v>
-      </c>
       <c r="G250" t="b">
-        <v>1</v>
-      </c>
-      <c r="H250" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:41" x14ac:dyDescent="0.35">
@@ -18744,14 +18447,8 @@
       <c r="E253" t="s">
         <v>498</v>
       </c>
-      <c r="F253" s="2">
-        <v>44541</v>
-      </c>
       <c r="G253" t="b">
-        <v>1</v>
-      </c>
-      <c r="H253" s="3">
-        <v>42460</v>
+        <v>0</v>
       </c>
     </row>
     <row r="254" spans="1:41" x14ac:dyDescent="0.35">
@@ -18858,14 +18555,8 @@
       <c r="E256" t="s">
         <v>247</v>
       </c>
-      <c r="F256" s="2">
-        <v>44541</v>
-      </c>
       <c r="G256" t="b">
-        <v>1</v>
-      </c>
-      <c r="H256" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="257" spans="1:43" x14ac:dyDescent="0.35">
@@ -18884,14 +18575,8 @@
       <c r="E257" t="s">
         <v>504</v>
       </c>
-      <c r="F257" s="2">
-        <v>44541</v>
-      </c>
       <c r="G257" t="b">
-        <v>1</v>
-      </c>
-      <c r="H257" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="258" spans="1:43" x14ac:dyDescent="0.35">
@@ -18910,14 +18595,8 @@
       <c r="E258" t="s">
         <v>506</v>
       </c>
-      <c r="F258" s="2">
-        <v>44541</v>
-      </c>
       <c r="G258" t="b">
-        <v>1</v>
-      </c>
-      <c r="H258" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="259" spans="1:43" x14ac:dyDescent="0.35">
@@ -18936,14 +18615,8 @@
       <c r="E259" t="s">
         <v>508</v>
       </c>
-      <c r="F259" s="2">
-        <v>44541</v>
-      </c>
       <c r="G259" t="b">
-        <v>1</v>
-      </c>
-      <c r="H259" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="260" spans="1:43" x14ac:dyDescent="0.35">
@@ -19538,7 +19211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A265" s="1">
         <v>2763</v>
       </c>
@@ -19558,7 +19231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A266" s="1">
         <v>2764</v>
       </c>
@@ -19578,7 +19251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A267" s="1">
         <v>2765</v>
       </c>
@@ -19614,14 +19287,8 @@
       <c r="E268" t="s">
         <v>525</v>
       </c>
-      <c r="F268" s="2">
-        <v>44541</v>
-      </c>
       <c r="G268" t="b">
-        <v>1</v>
-      </c>
-      <c r="H268" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="269" spans="1:43" x14ac:dyDescent="0.35">
@@ -19640,14 +19307,8 @@
       <c r="E269" t="s">
         <v>527</v>
       </c>
-      <c r="F269" s="2">
-        <v>44541</v>
-      </c>
       <c r="G269" t="b">
-        <v>1</v>
-      </c>
-      <c r="H269" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="270" spans="1:43" x14ac:dyDescent="0.35">
@@ -19666,14 +19327,8 @@
       <c r="E270" t="s">
         <v>529</v>
       </c>
-      <c r="F270" s="2">
-        <v>44541</v>
-      </c>
       <c r="G270" t="b">
-        <v>1</v>
-      </c>
-      <c r="H270" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="271" spans="1:43" x14ac:dyDescent="0.35">
@@ -19692,14 +19347,8 @@
       <c r="E271" t="s">
         <v>438</v>
       </c>
-      <c r="F271" s="2">
-        <v>44541</v>
-      </c>
       <c r="G271" t="b">
-        <v>1</v>
-      </c>
-      <c r="H271" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="272" spans="1:43" x14ac:dyDescent="0.35">
@@ -20117,14 +19766,8 @@
       <c r="E278" t="s">
         <v>540</v>
       </c>
-      <c r="F278" s="2">
-        <v>44541</v>
-      </c>
       <c r="G278" t="b">
-        <v>1</v>
-      </c>
-      <c r="H278" s="3">
-        <v>42460</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:43" x14ac:dyDescent="0.35">
@@ -20143,14 +19786,8 @@
       <c r="E279" t="s">
         <v>543</v>
       </c>
-      <c r="F279" s="2">
-        <v>44541</v>
-      </c>
       <c r="G279" t="b">
-        <v>1</v>
-      </c>
-      <c r="H279" s="3">
-        <v>41729</v>
+        <v>0</v>
       </c>
     </row>
     <row r="280" spans="1:43" x14ac:dyDescent="0.35">
@@ -20169,14 +19806,8 @@
       <c r="E280" t="s">
         <v>186</v>
       </c>
-      <c r="F280" s="2">
-        <v>44541</v>
-      </c>
       <c r="G280" t="b">
-        <v>1</v>
-      </c>
-      <c r="H280" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="281" spans="1:43" x14ac:dyDescent="0.35">
@@ -20195,14 +19826,8 @@
       <c r="E281" t="s">
         <v>546</v>
       </c>
-      <c r="F281" s="2">
-        <v>44541</v>
-      </c>
       <c r="G281" t="b">
-        <v>1</v>
-      </c>
-      <c r="H281" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="282" spans="1:43" x14ac:dyDescent="0.35">
@@ -20221,14 +19846,8 @@
       <c r="E282" t="s">
         <v>548</v>
       </c>
-      <c r="F282" s="2">
-        <v>44541</v>
-      </c>
       <c r="G282" t="b">
-        <v>1</v>
-      </c>
-      <c r="H282" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="283" spans="1:43" x14ac:dyDescent="0.35">
@@ -20247,14 +19866,8 @@
       <c r="E283" t="s">
         <v>548</v>
       </c>
-      <c r="F283" s="2">
-        <v>44541</v>
-      </c>
       <c r="G283" t="b">
-        <v>1</v>
-      </c>
-      <c r="H283" s="3">
-        <v>42094</v>
+        <v>0</v>
       </c>
     </row>
     <row r="284" spans="1:43" x14ac:dyDescent="0.35">
@@ -20273,14 +19886,8 @@
       <c r="E284" t="s">
         <v>548</v>
       </c>
-      <c r="F284" s="2">
-        <v>44541</v>
-      </c>
       <c r="G284" t="b">
-        <v>1</v>
-      </c>
-      <c r="H284" s="3">
-        <v>42460</v>
+        <v>0</v>
       </c>
     </row>
     <row r="285" spans="1:43" x14ac:dyDescent="0.35">
@@ -20512,14 +20119,8 @@
       <c r="E288" t="s">
         <v>558</v>
       </c>
-      <c r="F288" s="2">
-        <v>44541</v>
-      </c>
       <c r="G288" t="b">
-        <v>1</v>
-      </c>
-      <c r="H288" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="289" spans="1:43" x14ac:dyDescent="0.35">
@@ -21661,14 +21262,8 @@
       <c r="E300" t="s">
         <v>580</v>
       </c>
-      <c r="F300" s="2">
-        <v>44541</v>
-      </c>
       <c r="G300" t="b">
-        <v>1</v>
-      </c>
-      <c r="H300" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="301" spans="1:43" x14ac:dyDescent="0.35">
@@ -21687,14 +21282,8 @@
       <c r="E301" t="s">
         <v>582</v>
       </c>
-      <c r="F301" s="2">
-        <v>44541</v>
-      </c>
       <c r="G301" t="b">
-        <v>1</v>
-      </c>
-      <c r="H301" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="302" spans="1:43" x14ac:dyDescent="0.35">
@@ -21713,14 +21302,8 @@
       <c r="E302" t="s">
         <v>584</v>
       </c>
-      <c r="F302" s="2">
-        <v>44541</v>
-      </c>
       <c r="G302" t="b">
-        <v>1</v>
-      </c>
-      <c r="H302" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="303" spans="1:43" x14ac:dyDescent="0.35">
@@ -23261,7 +22844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A319" s="1">
         <v>2817</v>
       </c>
@@ -23281,7 +22864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A320" s="1">
         <v>2818</v>
       </c>
@@ -23301,7 +22884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:41" hidden="1" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A321" s="1">
         <v>2819</v>
       </c>
@@ -23321,7 +22904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:41" hidden="1" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A322" s="1">
         <v>2820</v>
       </c>
@@ -23738,7 +23321,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="331" spans="1:41" hidden="1" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A331" s="1">
         <v>2829</v>
       </c>
@@ -23774,14 +23357,8 @@
       <c r="E332" t="s">
         <v>635</v>
       </c>
-      <c r="F332" s="2">
-        <v>44541</v>
-      </c>
       <c r="G332" t="b">
-        <v>1</v>
-      </c>
-      <c r="H332" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="333" spans="1:41" x14ac:dyDescent="0.35">
@@ -23800,14 +23377,8 @@
       <c r="E333" t="s">
         <v>637</v>
       </c>
-      <c r="F333" s="2">
-        <v>44541</v>
-      </c>
       <c r="G333" t="b">
-        <v>1</v>
-      </c>
-      <c r="H333" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="334" spans="1:41" x14ac:dyDescent="0.35">
@@ -23826,14 +23397,8 @@
       <c r="E334" t="s">
         <v>639</v>
       </c>
-      <c r="F334" s="2">
-        <v>44541</v>
-      </c>
       <c r="G334" t="b">
-        <v>1</v>
-      </c>
-      <c r="H334" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="335" spans="1:41" x14ac:dyDescent="0.35">
@@ -23852,14 +23417,8 @@
       <c r="E335" t="s">
         <v>641</v>
       </c>
-      <c r="F335" s="2">
-        <v>44541</v>
-      </c>
       <c r="G335" t="b">
-        <v>1</v>
-      </c>
-      <c r="H335" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="336" spans="1:41" x14ac:dyDescent="0.35">
@@ -23878,14 +23437,8 @@
       <c r="E336" t="s">
         <v>643</v>
       </c>
-      <c r="F336" s="2">
-        <v>44541</v>
-      </c>
       <c r="G336" t="b">
-        <v>1</v>
-      </c>
-      <c r="H336" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="337" spans="1:43" x14ac:dyDescent="0.35">
@@ -24081,14 +23634,8 @@
       <c r="E340" t="s">
         <v>651</v>
       </c>
-      <c r="F340" s="2">
-        <v>44541</v>
-      </c>
       <c r="G340" t="b">
-        <v>1</v>
-      </c>
-      <c r="H340" s="3">
-        <v>42460</v>
+        <v>0</v>
       </c>
     </row>
     <row r="341" spans="1:43" x14ac:dyDescent="0.35">
@@ -24151,14 +23698,8 @@
       <c r="E342" t="s">
         <v>655</v>
       </c>
-      <c r="F342" s="2">
-        <v>44541</v>
-      </c>
       <c r="G342" t="b">
-        <v>1</v>
-      </c>
-      <c r="H342" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="343" spans="1:43" x14ac:dyDescent="0.35">
@@ -24177,14 +23718,8 @@
       <c r="E343" t="s">
         <v>249</v>
       </c>
-      <c r="F343" s="2">
-        <v>44541</v>
-      </c>
       <c r="G343" t="b">
-        <v>1</v>
-      </c>
-      <c r="H343" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="344" spans="1:43" x14ac:dyDescent="0.35">
@@ -24203,14 +23738,8 @@
       <c r="E344" t="s">
         <v>658</v>
       </c>
-      <c r="F344" s="2">
-        <v>44541</v>
-      </c>
       <c r="G344" t="b">
-        <v>1</v>
-      </c>
-      <c r="H344" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="345" spans="1:43" x14ac:dyDescent="0.35">
@@ -27116,7 +26645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A376" s="1">
         <v>2874</v>
       </c>
@@ -27136,7 +26665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A377" s="1">
         <v>2875</v>
       </c>
@@ -27156,7 +26685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A378" s="1">
         <v>2876</v>
       </c>
@@ -27176,7 +26705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A379" s="1">
         <v>2877</v>
       </c>
@@ -27383,14 +26912,8 @@
       <c r="E383" t="s">
         <v>734</v>
       </c>
-      <c r="F383" s="2">
-        <v>44541</v>
-      </c>
       <c r="G383" t="b">
-        <v>1</v>
-      </c>
-      <c r="H383" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="384" spans="1:43" x14ac:dyDescent="0.35">
@@ -27409,14 +26932,8 @@
       <c r="E384" t="s">
         <v>736</v>
       </c>
-      <c r="F384" s="2">
-        <v>44541</v>
-      </c>
       <c r="G384" t="b">
-        <v>1</v>
-      </c>
-      <c r="H384" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="385" spans="1:43" x14ac:dyDescent="0.35">
@@ -27435,14 +26952,8 @@
       <c r="E385" t="s">
         <v>738</v>
       </c>
-      <c r="F385" s="2">
-        <v>44541</v>
-      </c>
       <c r="G385" t="b">
-        <v>1</v>
-      </c>
-      <c r="H385" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="386" spans="1:43" x14ac:dyDescent="0.35">
@@ -27461,14 +26972,8 @@
       <c r="E386" t="s">
         <v>73</v>
       </c>
-      <c r="F386" s="2">
-        <v>44541</v>
-      </c>
       <c r="G386" t="b">
-        <v>1</v>
-      </c>
-      <c r="H386" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="387" spans="1:43" x14ac:dyDescent="0.35">
@@ -27596,14 +27101,8 @@
       <c r="E389" t="s">
         <v>744</v>
       </c>
-      <c r="F389" s="2">
-        <v>44541</v>
-      </c>
       <c r="G389" t="b">
-        <v>1</v>
-      </c>
-      <c r="H389" s="3">
-        <v>42094</v>
+        <v>0</v>
       </c>
     </row>
     <row r="390" spans="1:43" x14ac:dyDescent="0.35">
@@ -27622,14 +27121,8 @@
       <c r="E390" t="s">
         <v>744</v>
       </c>
-      <c r="F390" s="2">
-        <v>44541</v>
-      </c>
       <c r="G390" t="b">
-        <v>1</v>
-      </c>
-      <c r="H390" s="3">
-        <v>42094</v>
+        <v>0</v>
       </c>
     </row>
     <row r="391" spans="1:43" x14ac:dyDescent="0.35">
@@ -27648,14 +27141,8 @@
       <c r="E391" t="s">
         <v>747</v>
       </c>
-      <c r="F391" s="2">
-        <v>44541</v>
-      </c>
       <c r="G391" t="b">
-        <v>1</v>
-      </c>
-      <c r="H391" s="3">
-        <v>42460</v>
+        <v>0</v>
       </c>
     </row>
     <row r="392" spans="1:43" x14ac:dyDescent="0.35">
@@ -27674,14 +27161,8 @@
       <c r="E392" t="s">
         <v>747</v>
       </c>
-      <c r="F392" s="2">
-        <v>44541</v>
-      </c>
       <c r="G392" t="b">
-        <v>1</v>
-      </c>
-      <c r="H392" s="3">
-        <v>42460</v>
+        <v>0</v>
       </c>
     </row>
     <row r="393" spans="1:43" x14ac:dyDescent="0.35">
@@ -28685,14 +28166,8 @@
       <c r="E401" t="s">
         <v>766</v>
       </c>
-      <c r="F401" s="2">
-        <v>44541</v>
-      </c>
       <c r="G401" t="b">
-        <v>1</v>
-      </c>
-      <c r="H401" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="402" spans="1:43" x14ac:dyDescent="0.35">
@@ -28711,14 +28186,8 @@
       <c r="E402" t="s">
         <v>707</v>
       </c>
-      <c r="F402" s="2">
-        <v>44541</v>
-      </c>
       <c r="G402" t="b">
-        <v>1</v>
-      </c>
-      <c r="H402" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="403" spans="1:43" x14ac:dyDescent="0.35">
@@ -28737,14 +28206,8 @@
       <c r="E403" t="s">
         <v>769</v>
       </c>
-      <c r="F403" s="2">
-        <v>44541</v>
-      </c>
       <c r="G403" t="b">
-        <v>1</v>
-      </c>
-      <c r="H403" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="404" spans="1:43" x14ac:dyDescent="0.35">
@@ -29610,14 +29073,8 @@
       <c r="E412" t="s">
         <v>786</v>
       </c>
-      <c r="F412" s="2">
-        <v>44541</v>
-      </c>
       <c r="G412" t="b">
-        <v>1</v>
-      </c>
-      <c r="H412" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="413" spans="1:43" x14ac:dyDescent="0.35">
@@ -29636,14 +29093,8 @@
       <c r="E413" t="s">
         <v>788</v>
       </c>
-      <c r="F413" s="2">
-        <v>44541</v>
-      </c>
       <c r="G413" t="b">
-        <v>1</v>
-      </c>
-      <c r="H413" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="414" spans="1:43" x14ac:dyDescent="0.35">
@@ -29662,14 +29113,8 @@
       <c r="E414" t="s">
         <v>504</v>
       </c>
-      <c r="F414" s="2">
-        <v>44541</v>
-      </c>
       <c r="G414" t="b">
-        <v>1</v>
-      </c>
-      <c r="H414" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="415" spans="1:43" x14ac:dyDescent="0.35">
@@ -30979,14 +30424,8 @@
       <c r="E429" t="s">
         <v>820</v>
       </c>
-      <c r="F429" s="2">
-        <v>44541</v>
-      </c>
       <c r="G429" t="b">
-        <v>1</v>
-      </c>
-      <c r="H429" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="430" spans="1:43" x14ac:dyDescent="0.35">
@@ -31005,14 +30444,8 @@
       <c r="E430" t="s">
         <v>822</v>
       </c>
-      <c r="F430" s="2">
-        <v>44541</v>
-      </c>
       <c r="G430" t="b">
-        <v>1</v>
-      </c>
-      <c r="H430" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="431" spans="1:43" x14ac:dyDescent="0.35">
@@ -31031,14 +30464,8 @@
       <c r="E431" t="s">
         <v>824</v>
       </c>
-      <c r="F431" s="2">
-        <v>44541</v>
-      </c>
       <c r="G431" t="b">
-        <v>1</v>
-      </c>
-      <c r="H431" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="432" spans="1:43" x14ac:dyDescent="0.35">
@@ -31057,14 +30484,8 @@
       <c r="E432" t="s">
         <v>826</v>
       </c>
-      <c r="F432" s="2">
-        <v>44541</v>
-      </c>
       <c r="G432" t="b">
-        <v>1</v>
-      </c>
-      <c r="H432" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="433" spans="1:43" x14ac:dyDescent="0.35">
@@ -31083,14 +30504,8 @@
       <c r="E433" t="s">
         <v>824</v>
       </c>
-      <c r="F433" s="2">
-        <v>44541</v>
-      </c>
       <c r="G433" t="b">
-        <v>1</v>
-      </c>
-      <c r="H433" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="434" spans="1:43" x14ac:dyDescent="0.35">
@@ -31109,14 +30524,8 @@
       <c r="E434" t="s">
         <v>830</v>
       </c>
-      <c r="F434" s="2">
-        <v>44541</v>
-      </c>
       <c r="G434" t="b">
-        <v>1</v>
-      </c>
-      <c r="H434" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="435" spans="1:43" x14ac:dyDescent="0.35">
@@ -31135,14 +30544,8 @@
       <c r="E435" t="s">
         <v>832</v>
       </c>
-      <c r="F435" s="2">
-        <v>44541</v>
-      </c>
       <c r="G435" t="b">
-        <v>1</v>
-      </c>
-      <c r="H435" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="436" spans="1:43" x14ac:dyDescent="0.35">
@@ -31161,14 +30564,8 @@
       <c r="E436" t="s">
         <v>834</v>
       </c>
-      <c r="F436" s="2">
-        <v>44541</v>
-      </c>
       <c r="G436" t="b">
-        <v>1</v>
-      </c>
-      <c r="H436" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="437" spans="1:43" x14ac:dyDescent="0.35">
@@ -34172,14 +33569,8 @@
       <c r="E473" t="s">
         <v>883</v>
       </c>
-      <c r="F473" s="2">
-        <v>44541</v>
-      </c>
       <c r="G473" t="b">
-        <v>1</v>
-      </c>
-      <c r="H473" s="3">
-        <v>40633</v>
+        <v>0</v>
       </c>
     </row>
     <row r="474" spans="1:43" x14ac:dyDescent="0.35">
@@ -35492,7 +34883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="484" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="484" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A484" s="1">
         <v>2982</v>
       </c>
@@ -35512,7 +34903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="485" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="485" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A485" s="1">
         <v>2983</v>
       </c>
@@ -35532,7 +34923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="486" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="486" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A486" s="1">
         <v>2984</v>
       </c>
@@ -35670,7 +35061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="489" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="489" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A489" s="1">
         <v>2987</v>
       </c>
@@ -35690,7 +35081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="490" spans="1:43" hidden="1" x14ac:dyDescent="0.35">
+    <row r="490" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A490" s="1">
         <v>2988</v>
       </c>
@@ -35726,14 +35117,8 @@
       <c r="E491" t="s">
         <v>883</v>
       </c>
-      <c r="F491" s="2">
-        <v>44541</v>
-      </c>
       <c r="G491" t="b">
-        <v>1</v>
-      </c>
-      <c r="H491" s="3">
-        <v>40633</v>
+        <v>0</v>
       </c>
     </row>
     <row r="492" spans="1:43" x14ac:dyDescent="0.35">
@@ -35840,14 +35225,8 @@
       <c r="E494" t="s">
         <v>930</v>
       </c>
-      <c r="F494" s="2">
-        <v>44541</v>
-      </c>
       <c r="G494" t="b">
-        <v>1</v>
-      </c>
-      <c r="H494" s="3">
-        <v>42825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="495" spans="1:43" x14ac:dyDescent="0.35">
@@ -35866,14 +35245,8 @@
       <c r="E495" t="s">
         <v>932</v>
       </c>
-      <c r="F495" s="2">
-        <v>44541</v>
-      </c>
       <c r="G495" t="b">
-        <v>1</v>
-      </c>
-      <c r="H495" s="3">
-        <v>43190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="496" spans="1:43" x14ac:dyDescent="0.35">
@@ -35892,14 +35265,8 @@
       <c r="E496" t="s">
         <v>934</v>
       </c>
-      <c r="F496" s="2">
-        <v>44541</v>
-      </c>
       <c r="G496" t="b">
-        <v>1</v>
-      </c>
-      <c r="H496" s="3">
-        <v>42460</v>
+        <v>0</v>
       </c>
     </row>
     <row r="497" spans="1:41" x14ac:dyDescent="0.35">
@@ -35918,14 +35285,8 @@
       <c r="E497" t="s">
         <v>936</v>
       </c>
-      <c r="F497" s="2">
-        <v>44541</v>
-      </c>
       <c r="G497" t="b">
-        <v>1</v>
-      </c>
-      <c r="H497" s="3">
-        <v>43921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="498" spans="1:41" x14ac:dyDescent="0.35">
@@ -35944,14 +35305,8 @@
       <c r="E498" t="s">
         <v>938</v>
       </c>
-      <c r="F498" s="2">
-        <v>44541</v>
-      </c>
       <c r="G498" t="b">
-        <v>1</v>
-      </c>
-      <c r="H498" s="3">
-        <v>42094</v>
+        <v>0</v>
       </c>
     </row>
     <row r="499" spans="1:41" x14ac:dyDescent="0.35">
@@ -35970,14 +35325,8 @@
       <c r="E499" t="s">
         <v>940</v>
       </c>
-      <c r="F499" s="2">
-        <v>44541</v>
-      </c>
       <c r="G499" t="b">
-        <v>1</v>
-      </c>
-      <c r="H499" s="3">
-        <v>43555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="500" spans="1:41" x14ac:dyDescent="0.35">
@@ -36099,13 +35448,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AQ501" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="TRUE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AQ501" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>